<commit_message>
Better cliff chart. Now cliff_chart.xlsx is linked to pptx.
Note for the future: Use Excel to first make a step chart. Then
paste it into ppt and grant ppt permission to link to the excel
file so that you can edit data from ppt.
</commit_message>
<xml_diff>
--- a/cliff_chart.xlsx
+++ b/cliff_chart.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>RMT</t>
   </si>
@@ -36,6 +37,9 @@
   </si>
   <si>
     <t>Number of processors</t>
+  </si>
+  <si>
+    <t>dRMT number of processors</t>
   </si>
 </sst>
 </file>
@@ -80,6 +84,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0432FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -102,68 +111,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Throughput vs.</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> number of processors</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -184,16 +132,28 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="63500" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0432FF"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0432FF"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="0432FF"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -208,19 +168,19 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.99</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.99</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.99</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4.0</c:v>
@@ -232,7 +192,7 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.99</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>6.0</c:v>
@@ -268,7 +228,7 @@
                   <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.99</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>12.0</c:v>
@@ -400,7 +360,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -410,151 +370,126 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="63500" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000">
+                  <a:alpha val="70000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.99</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.99</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.99</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.99</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11.99</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>15.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>0.142857142857143</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
                   <c:v>0.14</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29</c:v>
+                  <c:v>0.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.43</c:v>
+                  <c:v>0.86</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.571428571428571</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.57</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.714285714285714</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.71</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.857142857142857</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.86</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1.0</c:v>
@@ -563,51 +498,6 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -623,11 +513,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-571884080"/>
-        <c:axId val="-571882336"/>
+        <c:axId val="-485931632"/>
+        <c:axId val="-532441488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-571884080"/>
+        <c:axId val="-485931632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,12 +526,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -654,12 +539,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -667,13 +549,16 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -687,12 +572,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -711,10 +593,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -725,7 +604,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -740,12 +619,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-571882336"/>
+        <c:crossAx val="-532441488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-571882336"/>
+        <c:axId val="-532441488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,12 +633,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -772,7 +646,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -785,22 +659,29 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2800" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Packets</a:t>
                 </a:r>
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2800" b="1"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2800" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>per cycle</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -814,7 +695,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -838,10 +719,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -852,12 +730,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -867,7 +742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-571884080"/>
+        <c:crossAx val="-485931632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -881,7 +756,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.756976015581945"/>
+          <c:y val="0.590664955426827"/>
+          <c:w val="0.193622198231932"/>
+          <c:h val="0.0921544278330847"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -895,12 +779,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1508,21 +1389,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1802,20 +1685,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1823,10 +1706,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1834,11 +1720,13 @@
         <v>0.08</v>
       </c>
       <c r="C2" s="1">
-        <f>1/7</f>
-        <v>0.14285714285714285</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1846,19 +1734,27 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f>2-0.01</f>
-        <v>1.99</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1866,18 +1762,27 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="C5" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2.99</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>0.16666666666666666</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1885,22 +1790,27 @@
         <v>0.25</v>
       </c>
       <c r="C7" s="1">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>3.99</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>0.25</v>
       </c>
       <c r="C8" s="1">
-        <f>4/7</f>
-        <v>0.5714285714285714</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1908,10 +1818,13 @@
         <v>0.33</v>
       </c>
       <c r="C9" s="1">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1919,10 +1832,13 @@
         <v>0.33</v>
       </c>
       <c r="C10" s="1">
-        <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1930,21 +1846,27 @@
         <v>0.33</v>
       </c>
       <c r="C11" s="1">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>5.99</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1">
         <v>0.33</v>
       </c>
       <c r="C12" s="1">
-        <v>0.8571428571428571</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1952,10 +1874,13 @@
         <v>0.5</v>
       </c>
       <c r="C13" s="1">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1963,10 +1888,13 @@
         <v>0.5</v>
       </c>
       <c r="C14" s="1">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1974,10 +1902,13 @@
         <v>0.5</v>
       </c>
       <c r="C15" s="1">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1985,171 +1916,129 @@
         <v>0.5</v>
       </c>
       <c r="C16" s="1">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17" s="1">
         <v>0.5</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
       <c r="B18" s="1">
         <v>0.5</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9</v>
       </c>
       <c r="B19" s="1">
         <v>0.5</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10</v>
       </c>
       <c r="B20" s="1">
         <v>0.5</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
       <c r="B21" s="1">
         <v>0.5</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>11</v>
       </c>
       <c r="B22" s="1">
         <v>0.5</v>
       </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>11</v>
       </c>
       <c r="B23" s="1">
         <v>0.5</v>
       </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>11.99</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1">
         <v>0.5</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>12</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>13</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>14</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>14</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>15</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
       <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2158,6 +2047,20 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21:R27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit changes until hardware details slide
</commit_message>
<xml_diff>
--- a/cliff_chart.xlsx
+++ b/cliff_chart.xlsx
@@ -230,27 +230,6 @@
                 <c:pt idx="22">
                   <c:v>12.0</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>15.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -328,27 +307,6 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,30 +380,6 @@
                 <c:pt idx="6">
                   <c:v>7.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -474,30 +408,6 @@
                   <c:v>0.86</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -513,11 +423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-485931632"/>
-        <c:axId val="-532441488"/>
+        <c:axId val="1324937840"/>
+        <c:axId val="1311036400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-485931632"/>
+        <c:axId val="1324937840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,12 +529,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-532441488"/>
+        <c:crossAx val="1311036400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-532441488"/>
+        <c:axId val="1311036400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,7 +652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-485931632"/>
+        <c:crossAx val="1324937840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1685,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:D17"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1817,12 +1727,6 @@
       <c r="B9" s="1">
         <v>0.33</v>
       </c>
-      <c r="C9" s="1">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1831,12 +1735,6 @@
       <c r="B10" s="1">
         <v>0.33</v>
       </c>
-      <c r="C10" s="1">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1845,12 +1743,6 @@
       <c r="B11" s="1">
         <v>0.33</v>
       </c>
-      <c r="C11" s="1">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1859,12 +1751,6 @@
       <c r="B12" s="1">
         <v>0.33</v>
       </c>
-      <c r="C12" s="1">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1873,12 +1759,6 @@
       <c r="B13" s="1">
         <v>0.5</v>
       </c>
-      <c r="C13" s="1">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1887,12 +1767,6 @@
       <c r="B14" s="1">
         <v>0.5</v>
       </c>
-      <c r="C14" s="1">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1901,12 +1775,6 @@
       <c r="B15" s="1">
         <v>0.5</v>
       </c>
-      <c r="C15" s="1">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1915,12 +1783,6 @@
       <c r="B16" s="1">
         <v>0.5</v>
       </c>
-      <c r="C16" s="1">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1984,62 +1846,6 @@
       </c>
       <c r="B24" s="1">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>12</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>13</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>13</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>14</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>14</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>15</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>15</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done writing through until the end of the slides
</commit_message>
<xml_diff>
--- a/cliff_chart.xlsx
+++ b/cliff_chart.xlsx
@@ -122,7 +122,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -157,7 +157,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$C$2:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -230,12 +230,15 @@
                 <c:pt idx="22">
                   <c:v>12.0</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$D$2:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
@@ -307,6 +310,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -318,7 +324,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -355,7 +361,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$32</c:f>
+              <c:f>Sheet1!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
@@ -385,7 +391,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$32</c:f>
+              <c:f>Sheet1!$B$2:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
@@ -423,11 +429,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1324937840"/>
-        <c:axId val="1311036400"/>
+        <c:axId val="1413356144"/>
+        <c:axId val="1383363136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1324937840"/>
+        <c:axId val="1413356144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,12 +535,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1311036400"/>
+        <c:crossAx val="1383363136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1311036400"/>
+        <c:axId val="1383363136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,7 +658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1324937840"/>
+        <c:crossAx val="1413356144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1595,257 +1601,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B31"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
         <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>9</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>10</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>10</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>11</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>11</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>12</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>